<commit_message>
Update photo insert excel sheet
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D126D31-52D0-0B48-8BAE-042A0B39FE76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB335A6B-33CE-E74E-BFE9-5F02BEC597C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="20201003" sheetId="1" r:id="rId1"/>
+    <sheet name="20201004" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="14">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -434,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785F6C26-C8ED-334D-987C-DB46B8438649}">
   <dimension ref="A1:D195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="82" workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3177,4 +3178,409 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB8C8D7-036F-ED43-A6FA-1C20CB38AC16}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="114.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(101, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C26" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(102, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(103, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(104, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(105, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(106, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(107, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(108, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(109, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(110, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(111, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(112, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(113, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(114, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(115, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(116, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(117, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(118, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(119, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(120, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(121, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(122, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(123, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>124</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(124, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(125, 7, '0'), 'dish');</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update SQLs for inserting photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB335A6B-33CE-E74E-BFE9-5F02BEC597C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201763C4-6E4A-F449-A451-BD98C187794B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="1" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
     <sheet name="20201004" sheetId="2" r:id="rId2"/>
+    <sheet name="20201005" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="15">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -77,12 +79,15 @@
   <si>
     <t>146da2dc-0526-11eb-ba65-065a10bcba76</t>
   </si>
+  <si>
+    <t>cf526b35-07b2-11eb-ba65-065a10bcba76</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +97,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,8 +129,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +449,7 @@
   <dimension ref="A1:D195"/>
   <sheetViews>
     <sheetView zoomScale="82" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3184,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB8C8D7-036F-ED43-A6FA-1C20CB38AC16}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3583,4 +3596,363 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEE6844-51FA-2540-B2A1-6C2C805F5D42}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C13" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(19, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(20, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(22, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(23, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da2dc-0526-11eb-ba65-065a10bcba76'), LPAD(24, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54E2B64-9697-F042-981B-542C8A4D6EB1}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="116.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>133</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(133, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>134</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C14" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(134, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>135</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(135, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>136</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(136, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>137</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(137, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>138</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(138, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add SQL for inserting dish photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201763C4-6E4A-F449-A451-BD98C187794B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0E0D9-E0E3-6940-977A-AB8F763EF359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="15">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -3773,10 +3773,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54E2B64-9697-F042-981B-542C8A4D6EB1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3816,7 +3816,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C14" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <f t="shared" ref="C3:C27" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
         <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(134, 7, '0'), 'dish');</v>
       </c>
     </row>
@@ -3950,6 +3950,162 @@
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf526b35-07b2-11eb-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(22, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(23, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(24, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(25, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(26, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(27, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(28, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(29, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(30, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(31, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(32, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>33</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(33, 7, '0'), 'dish');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SQL for inserting restaurants
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D0E0D9-E0E3-6940-977A-AB8F763EF359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29AD1F0-94EE-1C43-8026-2AE86C8D162E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="4" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
     <sheet name="20201004" sheetId="2" r:id="rId2"/>
     <sheet name="20201005" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="20201006" sheetId="4" r:id="rId4"/>
+    <sheet name="20201008" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="19">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -81,6 +82,18 @@
   </si>
   <si>
     <t>cf526b35-07b2-11eb-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>cf52fcae-07b2-11eb-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>da053b13-ffb0-11ea-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>69199622-0964-11eb-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>6918c03b-0964-11eb-ba65-065a10bcba76</t>
   </si>
 </sst>
 </file>
@@ -3775,8 +3788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54E2B64-9697-F042-981B-542C8A4D6EB1}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4111,4 +4124,970 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E61C9D-5011-F248-9057-DC969B217A52}">
+  <dimension ref="A1:C79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="114.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(9, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(10, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(11, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(12, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(19, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(20, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(22, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(23, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(24, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(25, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(26, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(27, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('cf52fcae-07b2-11eb-ba65-065a10bcba76'), LPAD(28, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(19, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(20, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f696-ffb0-11ea-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(9, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(10, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(11, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(12, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053b13-ffb0-11ea-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>36</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(36, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f4ef-ffb0-11ea-ba65-065a10bcba76'), LPAD(37, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(9, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(10, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(11, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(12, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C79" si="1">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B67, "'), LPAD(", A67, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>17</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>18</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>1</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>3</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>7</v>
+      </c>
+      <c r="B78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add SQL for inserting photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29AD1F0-94EE-1C43-8026-2AE86C8D162E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B84677-D2B2-4B49-A4B1-D5F291244854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="4" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="20">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>6918c03b-0964-11eb-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>da04eaf1-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
 </sst>
 </file>
@@ -4128,10 +4131,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E61C9D-5011-F248-9057-DC969B217A52}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4939,7 +4942,7 @@
         <v>18</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C79" si="1">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B67, "'), LPAD(", A67, ", 7, '0'), 'dish'", ");")</f>
+        <f t="shared" ref="C67:C86" si="1">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B67, "'), LPAD(", A67, ", 7, '0'), 'dish'", ");")</f>
         <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('6918c03b-0964-11eb-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
       </c>
     </row>
@@ -5085,6 +5088,90 @@
       <c r="C79" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('69199622-0964-11eb-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>4</v>
+      </c>
+      <c r="B83" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>7</v>
+      </c>
+      <c r="B86" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04eaf1-ffb0-11ea-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update photo insert SQL generation excel
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B84677-D2B2-4B49-A4B1-D5F291244854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2DE69D-0D71-1A4B-88DE-F9132AE42D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="4" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="5" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="20201005" sheetId="3" r:id="rId3"/>
     <sheet name="20201006" sheetId="4" r:id="rId4"/>
     <sheet name="20201008" sheetId="5" r:id="rId5"/>
+    <sheet name="20201012" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="20">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -4133,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E61C9D-5011-F248-9057-DC969B217A52}">
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5177,4 +5178,186 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD035A-C3A6-BC4D-93EA-7CF549CEF6DF}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C14" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(19, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(20, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(22, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(23, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(24, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f9c7-ffb0-11ea-ba65-065a10bcba76'), LPAD(25, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add SQL for insert photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2DE69D-0D71-1A4B-88DE-F9132AE42D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD7274C-7CAE-FA44-ABF7-C350BDB90367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="5" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="6" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="20201006" sheetId="4" r:id="rId4"/>
     <sheet name="20201008" sheetId="5" r:id="rId5"/>
     <sheet name="20201012" sheetId="6" r:id="rId6"/>
+    <sheet name="20201013" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="20">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -5184,8 +5185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDD035A-C3A6-BC4D-93EA-7CF549CEF6DF}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5360,4 +5361,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D36B866-400B-2A48-9A7F-C4752A6F22FE}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="116.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>139</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(139, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>140</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C11" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(140, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>141</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(141, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>142</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(142, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>143</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(143, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>144</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(144, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>145</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(145, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>146</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(146, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>147</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(147, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>148</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(148, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SQL for adding photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD7274C-7CAE-FA44-ABF7-C350BDB90367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E4336A-AD61-0043-BAD7-C83237D47509}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="6" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="7" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="20201008" sheetId="5" r:id="rId5"/>
     <sheet name="20201012" sheetId="6" r:id="rId6"/>
     <sheet name="20201013" sheetId="7" r:id="rId7"/>
+    <sheet name="20201020" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="21">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -99,6 +100,9 @@
   </si>
   <si>
     <t>da04eaf1-ffb0-11ea-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>da053615-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
 </sst>
 </file>
@@ -5367,8 +5371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D36B866-400B-2A48-9A7F-C4752A6F22FE}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5511,4 +5515,249 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CA5974-63A1-1144-9355-4D0230C3FE1D}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(149, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C19" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(150, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>151</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(151, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>152</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(152, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>153</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(153, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>154</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(154, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>155</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(155, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>156</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(156, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>157</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(157, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(158, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>159</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f5c9-ffb0-11ea-ba65-065a10bcba76'), LPAD(159, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053615-ffb0-11ea-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053615-ffb0-11ea-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053615-ffb0-11ea-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053615-ffb0-11ea-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da053615-ffb0-11ea-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da67c-0526-11eb-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('146da67c-0526-11eb-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SQL for inserting photos
</commit_message>
<xml_diff>
--- a/Image_Insert_SQL_Generator.xlsx
+++ b/Image_Insert_SQL_Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yukitaka.maeda/Documents/personal/tokyo-takeout-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183B6EA9-FA31-C440-8BEB-FDFEDF981D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652A3CAB-189C-E643-AFBA-512A1304A7E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="7" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="8" xr2:uid="{D1990E34-D14D-F945-B413-FD3DCC79E7CB}"/>
   </bookViews>
   <sheets>
     <sheet name="20201003" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="20201012" sheetId="6" r:id="rId6"/>
     <sheet name="20201013" sheetId="7" r:id="rId7"/>
     <sheet name="20201020" sheetId="8" r:id="rId8"/>
+    <sheet name="20201026" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="23">
   <si>
     <t>da04f5c9-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
@@ -106,6 +107,9 @@
   </si>
   <si>
     <t>9187407e-12a7-11eb-ba65-065a10bcba76</t>
+  </si>
+  <si>
+    <t>da04f82c-ffb0-11ea-ba65-065a10bcba76</t>
   </si>
 </sst>
 </file>
@@ -5524,8 +5528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CA5974-63A1-1144-9355-4D0230C3FE1D}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5859,4 +5863,285 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D45398C-A363-E04E-99A6-E3D6B5E0ADA2}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B2, "'), LPAD(", A2, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(1, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C22" si="0">_xlfn.CONCAT("INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('", B3, "'), LPAD(", A3, ", 7, '0'), 'dish'", ");")</f>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(2, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(3, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(4, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(5, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(6, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(7, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(8, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(9, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(10, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(11, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(12, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(13, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(14, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(15, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(16, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(17, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(18, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(19, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(20, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO photos(restaurant_id, name, type) VALUES(UuidToBin('da04f82c-ffb0-11ea-ba65-065a10bcba76'), LPAD(21, 7, '0'), 'dish');</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>